<commit_message>
update bwaise summary tables, add env and instructions on reproducing the results
</commit_message>
<xml_diff>
--- a/exposan/bwaise/comparison/comparison_summary.xlsx
+++ b/exposan/bwaise/comparison/comparison_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/comparison/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Library/CloudStorage/OneDrive-Personal/Coding/es/exposan/bwaise/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="13_ncr:1_{A41B6D32-C405-4C4B-AC94-404E34509E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C352C85B-5E80-9D40-B4DB-EE4E5DA03E48}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD138D7-E58D-1F49-B19C-14CBE5164B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25020" yWindow="8920" windowWidth="25920" windowHeight="16060" xr2:uid="{C322E86D-AF8D-7D47-9916-FBB30EE50BE1}"/>
+    <workbookView xWindow="17560" yWindow="7100" windowWidth="25920" windowHeight="16060" xr2:uid="{C322E86D-AF8D-7D47-9916-FBB30EE50BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -339,10 +339,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -663,7 +663,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,26 +679,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="30"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -746,7 +746,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -796,7 +796,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -847,7 +847,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -871,7 +871,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -895,7 +895,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -945,7 +945,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
@@ -1216,14 +1216,14 @@
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="22">
-        <v>58.9</v>
+        <v>58.6</v>
       </c>
       <c r="D23" s="9">
         <v>59.03</v>
@@ -1243,7 +1243,7 @@
       <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
@@ -1377,16 +1377,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>